<commit_message>
just missing b exercises
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week3/work.xlsx
+++ b/PM2/econ/week3/work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD4A919-041F-419F-A318-977B97AE19D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430C4072-B623-4328-9B7B-D4849A5CFB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{FAF6C9F4-7133-4E64-911F-7351721DE4A5}"/>
   </bookViews>
@@ -159,7 +159,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -214,7 +214,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -642,7 +642,7 @@
         <v>20</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F9" si="3">$J$5</f>
+        <f t="shared" ref="F6:F8" si="3">$J$5</f>
         <v>0</v>
       </c>
       <c r="G6">
@@ -871,11 +871,11 @@
         <v>24</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E9" si="2">$K$2</f>
+        <f t="shared" ref="E6:E8" si="2">$K$2</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F9" si="3">$K$1</f>
+        <f t="shared" ref="F6:F8" si="3">$K$1</f>
         <v>0</v>
       </c>
       <c r="G6">
@@ -1092,7 +1092,7 @@
         <v>24</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E8" si="2">$C$11</f>
+        <f t="shared" ref="E5:E7" si="2">$C$11</f>
         <v>0</v>
       </c>
       <c r="F5">
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F5:F8" si="5">$C$12</f>
+        <f t="shared" ref="F6:F7" si="5">$C$12</f>
         <v>0</v>
       </c>
       <c r="G6">

</xml_diff>